<commit_message>
Added a project recording video, passport size image and changed the readme of the project for better communication
</commit_message>
<xml_diff>
--- a/0.2 Data Dictionary.xlsx
+++ b/0.2 Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Bank Loan Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510CDDC0-3334-4B6F-95FD-086B7810E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C5406-08BE-4051-9F5D-57CBFF6A052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_dictionary" sheetId="1" r:id="rId1"/>
@@ -685,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="130.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -998,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F4A93-FA65-4873-9993-AA8576A19D12}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>